<commit_message>
Ugentlig opdatering af tidsplan iht. møde.
</commit_message>
<xml_diff>
--- a/01 Adminstration/04 Tidsplan.xlsx
+++ b/01 Adminstration/04 Tidsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp-cl\Desktop\Uni\5 Semester\P5\GIT\ESD_P5\01 Adminstration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49747FA-DC84-42E9-8996-0FD60C7B12BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60195237-D029-407E-BD80-A7ED6D9EE0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69133E36-BD8C-42CB-86D0-28FF962A2138}"/>
   </bookViews>
@@ -904,7 +904,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,10 +1015,10 @@
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
@@ -1105,7 +1105,7 @@
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
-      <c r="H9" s="8"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1145,7 +1145,7 @@
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
       <c r="G11" s="31"/>
-      <c r="H11" s="20"/>
+      <c r="H11" s="31"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
@@ -1565,6 +1565,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9eb01566-652b-4477-b28c-3e66da18d344">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1ef46024-2ca0-4db1-9ed8-b314520bddf3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100FE580F2D3026B143BDF291C5137D2DA0" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="cbf9c7ba37e5329923f2631dbd7f57d0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9eb01566-652b-4477-b28c-3e66da18d344" xmlns:ns3="1ef46024-2ca0-4db1-9ed8-b314520bddf3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51e2ef3359a75a136c9bc01b553e9c72" ns2:_="" ns3:_="">
     <xsd:import namespace="9eb01566-652b-4477-b28c-3e66da18d344"/>
@@ -1771,27 +1791,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4288EBCF-420A-4A04-9E3C-0310870484B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="48223c98-16c9-41d7-8092-c9ed2a69b2b9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5fbc24e0-ed7e-44d1-93b2-2d3381b4859a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9eb01566-652b-4477-b28c-3e66da18d344"/>
+    <ds:schemaRef ds:uri="1ef46024-2ca0-4db1-9ed8-b314520bddf3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9eb01566-652b-4477-b28c-3e66da18d344">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1ef46024-2ca0-4db1-9ed8-b314520bddf3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CF982C2-996F-4141-9385-FFB5C146D1F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BED2C824-EE10-4B11-9501-FDAC8E8CEC63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1810,33 +1837,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CF982C2-996F-4141-9385-FFB5C146D1F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4288EBCF-420A-4A04-9E3C-0310870484B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="48223c98-16c9-41d7-8092-c9ed2a69b2b9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5fbc24e0-ed7e-44d1-93b2-2d3381b4859a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9eb01566-652b-4477-b28c-3e66da18d344"/>
-    <ds:schemaRef ds:uri="1ef46024-2ca0-4db1-9ed8-b314520bddf3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f5dbba49-ce06-496f-ac3e-0cf14361d934}" enabled="0" method="" siteId="{f5dbba49-ce06-496f-ac3e-0cf14361d934}" removed="1"/>

</xml_diff>

<commit_message>
Opdatering af tidsplan iht. dagligt møde
</commit_message>
<xml_diff>
--- a/01 Adminstration/04 Tidsplan.xlsx
+++ b/01 Adminstration/04 Tidsplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp-cl\Desktop\Uni\5 Semester\P5\GIT\ESD_P5\01 Adminstration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60195237-D029-407E-BD80-A7ED6D9EE0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC75D416-6AC4-4C08-AFB4-FECA77C014AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69133E36-BD8C-42CB-86D0-28FF962A2138}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Plan</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>type sammen</t>
+  </si>
+  <si>
+    <t>Uge 46 slut enkelt udvikling, uge 47, samling</t>
   </si>
 </sst>
 </file>
@@ -904,7 +907,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1073,7 @@
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
@@ -1106,7 +1109,7 @@
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
-      <c r="I9" s="8"/>
+      <c r="I9" s="31"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -1146,7 +1149,7 @@
       <c r="F11" s="31"/>
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
-      <c r="I11" s="20"/>
+      <c r="I11" s="31"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
@@ -1394,7 +1397,9 @@
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="J27" s="22" t="s">
+        <v>35</v>
+      </c>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
       <c r="M27" s="22"/>
@@ -1565,26 +1570,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9eb01566-652b-4477-b28c-3e66da18d344">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1ef46024-2ca0-4db1-9ed8-b314520bddf3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100FE580F2D3026B143BDF291C5137D2DA0" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="cbf9c7ba37e5329923f2631dbd7f57d0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9eb01566-652b-4477-b28c-3e66da18d344" xmlns:ns3="1ef46024-2ca0-4db1-9ed8-b314520bddf3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51e2ef3359a75a136c9bc01b553e9c72" ns2:_="" ns3:_="">
     <xsd:import namespace="9eb01566-652b-4477-b28c-3e66da18d344"/>
@@ -1791,7 +1776,54 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9eb01566-652b-4477-b28c-3e66da18d344">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1ef46024-2ca0-4db1-9ed8-b314520bddf3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BED2C824-EE10-4B11-9501-FDAC8E8CEC63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9eb01566-652b-4477-b28c-3e66da18d344"/>
+    <ds:schemaRef ds:uri="1ef46024-2ca0-4db1-9ed8-b314520bddf3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CF982C2-996F-4141-9385-FFB5C146D1F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4288EBCF-420A-4A04-9E3C-0310870484B1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="48223c98-16c9-41d7-8092-c9ed2a69b2b9"/>
@@ -1810,33 +1842,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CF982C2-996F-4141-9385-FFB5C146D1F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BED2C824-EE10-4B11-9501-FDAC8E8CEC63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9eb01566-652b-4477-b28c-3e66da18d344"/>
-    <ds:schemaRef ds:uri="1ef46024-2ca0-4db1-9ed8-b314520bddf3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f5dbba49-ce06-496f-ac3e-0cf14361d934}" enabled="0" method="" siteId="{f5dbba49-ce06-496f-ac3e-0cf14361d934}" removed="1"/>

</xml_diff>

<commit_message>
Opdatering af tidsplan iht. møde
</commit_message>
<xml_diff>
--- a/01 Adminstration/04 Tidsplan.xlsx
+++ b/01 Adminstration/04 Tidsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp-cl\Desktop\Uni\5 Semester\P5\GIT\ESD_P5\01 Adminstration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC75D416-6AC4-4C08-AFB4-FECA77C014AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916F135A-4BAF-429C-9729-9DC5ECCCA3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69133E36-BD8C-42CB-86D0-28FF962A2138}"/>
   </bookViews>
@@ -488,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,6 +585,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -907,7 +910,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,8 +1077,8 @@
       <c r="G7" s="20"/>
       <c r="H7" s="8"/>
       <c r="I7" s="31"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
@@ -1110,8 +1113,8 @@
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
       <c r="I9" s="31"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -1150,8 +1153,8 @@
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
       <c r="L11" s="20"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8" t="s">
@@ -1261,7 +1264,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+      <c r="K17" s="36"/>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
@@ -1570,6 +1573,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9eb01566-652b-4477-b28c-3e66da18d344">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1ef46024-2ca0-4db1-9ed8-b314520bddf3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100FE580F2D3026B143BDF291C5137D2DA0" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="cbf9c7ba37e5329923f2631dbd7f57d0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9eb01566-652b-4477-b28c-3e66da18d344" xmlns:ns3="1ef46024-2ca0-4db1-9ed8-b314520bddf3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51e2ef3359a75a136c9bc01b553e9c72" ns2:_="" ns3:_="">
     <xsd:import namespace="9eb01566-652b-4477-b28c-3e66da18d344"/>
@@ -1776,27 +1799,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4288EBCF-420A-4A04-9E3C-0310870484B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="48223c98-16c9-41d7-8092-c9ed2a69b2b9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5fbc24e0-ed7e-44d1-93b2-2d3381b4859a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9eb01566-652b-4477-b28c-3e66da18d344"/>
+    <ds:schemaRef ds:uri="1ef46024-2ca0-4db1-9ed8-b314520bddf3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9eb01566-652b-4477-b28c-3e66da18d344">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1ef46024-2ca0-4db1-9ed8-b314520bddf3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CF982C2-996F-4141-9385-FFB5C146D1F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BED2C824-EE10-4B11-9501-FDAC8E8CEC63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1815,33 +1845,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CF982C2-996F-4141-9385-FFB5C146D1F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4288EBCF-420A-4A04-9E3C-0310870484B1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="48223c98-16c9-41d7-8092-c9ed2a69b2b9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5fbc24e0-ed7e-44d1-93b2-2d3381b4859a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9eb01566-652b-4477-b28c-3e66da18d344"/>
-    <ds:schemaRef ds:uri="1ef46024-2ca0-4db1-9ed8-b314520bddf3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f5dbba49-ce06-496f-ac3e-0cf14361d934}" enabled="0" method="" siteId="{f5dbba49-ce06-496f-ac3e-0cf14361d934}" removed="1"/>

</xml_diff>